<commit_message>
Adjustet Projektplan to new classes
</commit_message>
<xml_diff>
--- a/Entwurf/Projektplan_new.xlsx
+++ b/Entwurf/Projektplan_new.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Shared\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,27 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
-    <t>MainWindow, FilterTab</t>
-  </si>
-  <si>
-    <t>FrameView</t>
-  </si>
-  <si>
-    <t>FilterList, FilterConfigurationLoader, FilterConfigurationSaver</t>
-  </si>
-  <si>
-    <t>YUVFileReader, YUV411FileReader, Compression, YUV411Vector</t>
-  </si>
-  <si>
-    <t>GraphWidget, Graph</t>
-  </si>
-  <si>
-    <t>VideoLoader, AVVideo</t>
-  </si>
-  <si>
-    <t>Video, VideoPlayer</t>
-  </si>
-  <si>
     <t>FilterApplier, 5 Ffmpeg Filter</t>
   </si>
   <si>
@@ -62,9 +41,6 @@
     <t>VideoConverter</t>
   </si>
   <si>
-    <t>Timer, ControlPanel, PlayerControlPanel, PreviewControlPanel</t>
-  </si>
-  <si>
     <t>YUV422Reader, YUV444Reader</t>
   </si>
   <si>
@@ -107,18 +83,12 @@
     <t>5 Filter Boxen</t>
   </si>
   <si>
-    <t>4 Filter Boxen</t>
-  </si>
-  <si>
     <t xml:space="preserve">MainWindowMemento, FilterTabMemento, AnalysisTabMemento </t>
   </si>
   <si>
     <t>Wunschkriterien Graphen</t>
   </si>
   <si>
-    <t>Undo / Redo Commands</t>
-  </si>
-  <si>
     <t>ProjectLoader, ProjectSaver</t>
   </si>
   <si>
@@ -129,6 +99,36 @@
   </si>
   <si>
     <t>Dauer</t>
+  </si>
+  <si>
+    <t>Video, Player, VideoPlayer, ForwardPlayer</t>
+  </si>
+  <si>
+    <t>Timer, ControlPanel, PlayerControlPanel, PreviewControlPanel, GlobalControlPanel</t>
+  </si>
+  <si>
+    <t>EncodedVideo, YuvVideo</t>
+  </si>
+  <si>
+    <t>MainWindow, FilterTab (Ben)</t>
+  </si>
+  <si>
+    <t>FrameView (Johannes)</t>
+  </si>
+  <si>
+    <t>FilterList, FilterConfigurationLoader, FilterConfigurationSaver (Noel)</t>
+  </si>
+  <si>
+    <t>YUVFileReader, YUV411FileReader, Compression, YUV411Vector, YuvType (Sascha)</t>
+  </si>
+  <si>
+    <t>GraphWidget, Graph (Carina)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> VideoLoader, AVVideo (Simon)</t>
+  </si>
+  <si>
+    <t>Undo / Redo Commands (alle)</t>
   </si>
 </sst>
 </file>
@@ -210,6 +210,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Projektplan</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -275,25 +300,25 @@
               <c:strCache>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>MainWindow, FilterTab</c:v>
+                  <c:v>MainWindow, FilterTab (Ben)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>FrameView</c:v>
+                  <c:v>FrameView (Johannes)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>FilterList, FilterConfigurationLoader, FilterConfigurationSaver</c:v>
+                  <c:v>FilterList, FilterConfigurationLoader, FilterConfigurationSaver (Noel)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>YUVFileReader, YUV411FileReader, Compression, YUV411Vector</c:v>
+                  <c:v>YUVFileReader, YUV411FileReader, Compression, YUV411Vector, YuvType (Sascha)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>GraphWidget, Graph</c:v>
+                  <c:v>GraphWidget, Graph (Carina)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>VideoLoader, AVVideo</c:v>
+                  <c:v> VideoLoader, AVVideo (Simon)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Video, VideoPlayer</c:v>
+                  <c:v>Video, Player, VideoPlayer, ForwardPlayer</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>FilterApplier, 5 Ffmpeg Filter</c:v>
@@ -311,7 +336,7 @@
                   <c:v>VideoConverter</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Timer, ControlPanel, PlayerControlPanel, PreviewControlPanel</c:v>
+                  <c:v>Timer, ControlPanel, PlayerControlPanel, PreviewControlPanel, GlobalControlPanel</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>YUV422Reader, YUV444Reader</c:v>
@@ -356,10 +381,10 @@
                   <c:v>YUV422FileSaver, YUV444FileSaver</c:v>
                 </c:pt>
                 <c:pt idx="27">
+                  <c:v>EncodedVideo, YuvVideo</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>5 Filter Boxen</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>4 Filter Boxen</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>MainWindowMemento, FilterTabMemento, AnalysisTabMemento </c:v>
@@ -368,7 +393,7 @@
                   <c:v>Wunschkriterien Graphen</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>Undo / Redo Commands</c:v>
+                  <c:v>Undo / Redo Commands (alle)</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>ProjectLoader, ProjectSaver</c:v>
@@ -383,103 +408,103 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="17">
-                  <c:v>8</c:v>
-                </c:pt>
                 <c:pt idx="18">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="26">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="23">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="29">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="30">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="29">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>13</c:v>
-                </c:pt>
                 <c:pt idx="31">
-                  <c:v>13</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>15</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -878,9 +903,26 @@
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="3000">
+                    <a:srgbClr val="7030A0"/>
+                  </a:gs>
+                  <a:gs pos="97000">
+                    <a:srgbClr val="FF0000"/>
+                  </a:gs>
+                  <a:gs pos="73000">
+                    <a:schemeClr val="accent2"/>
+                  </a:gs>
+                  <a:gs pos="29000">
+                    <a:srgbClr val="0070C0"/>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:srgbClr val="FFFF00"/>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="1"/>
+              </a:gradFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
@@ -907,25 +949,25 @@
               <c:strCache>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>MainWindow, FilterTab</c:v>
+                  <c:v>MainWindow, FilterTab (Ben)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>FrameView</c:v>
+                  <c:v>FrameView (Johannes)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>FilterList, FilterConfigurationLoader, FilterConfigurationSaver</c:v>
+                  <c:v>FilterList, FilterConfigurationLoader, FilterConfigurationSaver (Noel)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>YUVFileReader, YUV411FileReader, Compression, YUV411Vector</c:v>
+                  <c:v>YUVFileReader, YUV411FileReader, Compression, YUV411Vector, YuvType (Sascha)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>GraphWidget, Graph</c:v>
+                  <c:v>GraphWidget, Graph (Carina)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>VideoLoader, AVVideo</c:v>
+                  <c:v> VideoLoader, AVVideo (Simon)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Video, VideoPlayer</c:v>
+                  <c:v>Video, Player, VideoPlayer, ForwardPlayer</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>FilterApplier, 5 Ffmpeg Filter</c:v>
@@ -943,7 +985,7 @@
                   <c:v>VideoConverter</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Timer, ControlPanel, PlayerControlPanel, PreviewControlPanel</c:v>
+                  <c:v>Timer, ControlPanel, PlayerControlPanel, PreviewControlPanel, GlobalControlPanel</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>YUV422Reader, YUV444Reader</c:v>
@@ -988,10 +1030,10 @@
                   <c:v>YUV422FileSaver, YUV444FileSaver</c:v>
                 </c:pt>
                 <c:pt idx="27">
+                  <c:v>EncodedVideo, YuvVideo</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>5 Filter Boxen</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>4 Filter Boxen</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>MainWindowMemento, FilterTabMemento, AnalysisTabMemento </c:v>
@@ -1000,7 +1042,7 @@
                   <c:v>Wunschkriterien Graphen</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>Undo / Redo Commands</c:v>
+                  <c:v>Undo / Redo Commands (alle)</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>ProjectLoader, ProjectSaver</c:v>
@@ -1099,7 +1141,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>2</c:v>
@@ -1108,7 +1150,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>3</c:v>
@@ -1127,11 +1169,11 @@
         </c:dLbls>
         <c:gapWidth val="115"/>
         <c:overlap val="100"/>
-        <c:axId val="411003344"/>
-        <c:axId val="411010064"/>
+        <c:axId val="282528704"/>
+        <c:axId val="282529264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="411003344"/>
+        <c:axId val="282528704"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1174,7 +1216,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="411010064"/>
+        <c:crossAx val="282529264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1182,10 +1224,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="411010064"/>
+        <c:axId val="282529264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="1"/>
+          <c:max val="18"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1234,7 +1277,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="411003344"/>
+        <c:crossAx val="282528704"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1839,13 +1882,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
+      <xdr:colOff>683559</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>9524</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Diagramm 2"/>
+        <xdr:cNvPr id="3" name="Diagramm 2" descr="&#10;"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2128,32 +2171,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="74.42578125" customWidth="1"/>
+    <col min="1" max="1" width="75.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3">
         <v>0</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -2161,10 +2204,10 @@
     </row>
     <row r="4" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -2172,10 +2215,10 @@
     </row>
     <row r="5" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -2183,10 +2226,10 @@
     </row>
     <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -2194,10 +2237,10 @@
     </row>
     <row r="7" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -2205,10 +2248,10 @@
     </row>
     <row r="8" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -2216,10 +2259,10 @@
     </row>
     <row r="9" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -2227,10 +2270,10 @@
     </row>
     <row r="10" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <v>3</v>
@@ -2238,10 +2281,10 @@
     </row>
     <row r="11" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -2249,10 +2292,10 @@
     </row>
     <row r="12" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12">
         <v>4</v>
@@ -2260,10 +2303,10 @@
     </row>
     <row r="13" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13">
         <v>3</v>
@@ -2271,10 +2314,10 @@
     </row>
     <row r="14" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -2282,10 +2325,10 @@
     </row>
     <row r="15" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15">
         <v>3</v>
@@ -2293,10 +2336,10 @@
     </row>
     <row r="16" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B16">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16">
         <v>3</v>
@@ -2304,10 +2347,10 @@
     </row>
     <row r="17" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B17">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -2315,10 +2358,10 @@
     </row>
     <row r="18" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B18">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18">
         <v>4</v>
@@ -2326,10 +2369,10 @@
     </row>
     <row r="19" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B19">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19">
         <v>3</v>
@@ -2337,10 +2380,10 @@
     </row>
     <row r="20" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B20">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C20">
         <v>3</v>
@@ -2348,10 +2391,10 @@
     </row>
     <row r="21" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B21">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -2359,10 +2402,10 @@
     </row>
     <row r="22" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B22">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -2370,10 +2413,10 @@
     </row>
     <row r="23" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B23">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C23">
         <v>3</v>
@@ -2381,10 +2424,10 @@
     </row>
     <row r="24" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B24">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C24">
         <v>2</v>
@@ -2392,10 +2435,10 @@
     </row>
     <row r="25" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B25">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C25">
         <v>3</v>
@@ -2403,10 +2446,10 @@
     </row>
     <row r="26" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B26">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -2414,10 +2457,10 @@
     </row>
     <row r="27" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B27">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C27">
         <v>2</v>
@@ -2425,10 +2468,10 @@
     </row>
     <row r="28" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B28">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -2436,10 +2479,10 @@
     </row>
     <row r="29" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B29">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C29">
         <v>3</v>
@@ -2447,10 +2490,10 @@
     </row>
     <row r="30" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B30">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C30">
         <v>2</v>
@@ -2458,21 +2501,21 @@
     </row>
     <row r="31" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B31">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B32">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C32">
         <v>2</v>
@@ -2480,10 +2523,10 @@
     </row>
     <row r="33" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B33">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C33">
         <v>3</v>
@@ -2491,21 +2534,21 @@
     </row>
     <row r="34" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B34">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C34">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B35">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C35">
         <v>3</v>

</xml_diff>